<commit_message>
support for two env
</commit_message>
<xml_diff>
--- a/docs/app-port-2.xlsx
+++ b/docs/app-port-2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
   <si>
     <t>APP_NAME</t>
   </si>
@@ -155,6 +155,12 @@
     <t>UBX</t>
   </si>
   <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>192.168.143.4</t>
+  </si>
+  <si>
     <t>Sun</t>
   </si>
   <si>
@@ -164,13 +170,19 @@
     <t>Thing</t>
   </si>
   <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>K8s</t>
+  </si>
+  <si>
+    <t>192.168.143.4-5</t>
+  </si>
+  <si>
     <t>FULL</t>
   </si>
   <si>
     <t>凭证</t>
-  </si>
-  <si>
-    <t>K8s</t>
   </si>
   <si>
     <t>FULL-1</t>
@@ -913,7 +925,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -933,6 +945,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1257,10 +1272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6"/>
@@ -1274,6 +1289,7 @@
     <col min="8" max="8" width="13.8666666666667" customWidth="1"/>
     <col min="9" max="9" width="14.9333333333333" customWidth="1"/>
     <col min="10" max="10" width="13.8666666666667" customWidth="1"/>
+    <col min="13" max="13" width="21.1083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="2:4">
@@ -1598,7 +1614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" customFormat="1" spans="1:8">
+    <row r="28" customFormat="1" spans="1:13">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1617,10 +1633,22 @@
       <c r="H28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" customFormat="1" spans="1:8">
+      <c r="J28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28">
+        <v>8082</v>
+      </c>
+      <c r="M28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="1" spans="1:13">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1629,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G29">
         <v>8092</v>
@@ -1637,10 +1665,20 @@
       <c r="H29" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="J29" s="8"/>
+      <c r="K29" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29">
+        <v>8081</v>
+      </c>
+      <c r="M29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1648,18 +1686,42 @@
       <c r="C30">
         <v>2</v>
       </c>
+      <c r="J30" s="8"/>
+      <c r="K30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30">
+        <v>8083</v>
+      </c>
+      <c r="M30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="10:13">
+      <c r="J31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K31" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31">
+        <v>8085</v>
+      </c>
+      <c r="M31" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="7:8">
       <c r="G32" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
@@ -1671,10 +1733,10 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:8">
@@ -1689,10 +1751,10 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H34" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:8">
@@ -1707,10 +1769,10 @@
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="2:5">
@@ -1719,7 +1781,7 @@
         <v>22</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1731,7 +1793,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -1743,7 +1805,7 @@
         <v>22</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -1766,7 +1828,7 @@
         <v>14</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -1782,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E44" s="5">
         <v>8082</v>
@@ -1807,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E45" s="4">
         <v>8082</v>
@@ -1832,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E46" s="5">
         <v>8082</v>
@@ -1857,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E47" s="6">
         <v>8082</v>
@@ -1893,15 +1955,16 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D51">
         <v>8084</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B33:B38"/>
+    <mergeCell ref="J28:J30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>